<commit_message>
menü oluşturma ve adetler tamam
</commit_message>
<xml_diff>
--- a/data/db tasarım.xlsx
+++ b/data/db tasarım.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Baris\Desktop\MVC\HamburgerProje\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D374CB0C-145B-4ECA-9D39-FF8846B532D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FA924E-C790-4E05-838B-4561D48B03DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,12 +210,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:Z40"/>
+  <dimension ref="A4:W24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,23 +510,24 @@
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="27" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -536,29 +535,29 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="H4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="O4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="V4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
       <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -574,53 +573,53 @@
       <c r="E5" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="G5" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="H5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="J5" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="K5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="1" t="s">
+      <c r="S5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="V5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="W5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="V5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z5" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -632,41 +631,41 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="H6" s="1">
+      <c r="G6" s="1">
         <v>1</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="1">
+      <c r="I6" s="1">
         <v>20</v>
       </c>
+      <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="O6" s="1">
+        <v>3</v>
+      </c>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="S6" s="1">
         <v>1</v>
       </c>
-      <c r="P6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>3</v>
-      </c>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="V6" s="1">
-        <v>1</v>
-      </c>
-      <c r="W6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="X6" s="1">
+      <c r="U6" s="1">
         <v>15</v>
       </c>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -678,41 +677,41 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="H7" s="1">
-        <v>2</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="1">
+      <c r="I7" s="1">
         <v>20</v>
       </c>
+      <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="M7" s="1">
+        <v>2</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="O7" s="1">
-        <v>2</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>3</v>
-      </c>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="V7" s="1">
-        <v>2</v>
-      </c>
-      <c r="W7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="S7" s="1">
+        <v>2</v>
+      </c>
+      <c r="T7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="X7" s="1">
+      <c r="U7" s="1">
         <v>15</v>
       </c>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -724,61 +723,61 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="H8" s="1">
-        <v>3</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="G8" s="1">
+        <v>3</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="1">
+      <c r="I8" s="1">
         <v>15</v>
       </c>
+      <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="M8" s="1">
+        <v>3</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="O8" s="1">
         <v>3</v>
       </c>
-      <c r="P8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>3</v>
-      </c>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="V8" s="1">
-        <v>3</v>
-      </c>
-      <c r="W8" s="1" t="s">
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="S8" s="1">
+        <v>3</v>
+      </c>
+      <c r="T8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="X8" s="1">
+      <c r="U8" s="1">
         <v>15</v>
       </c>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="V9" s="1">
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="S9" s="1">
         <v>4</v>
       </c>
-      <c r="W9" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="X9" s="1">
+      <c r="U9" s="1">
         <v>10</v>
       </c>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>0</v>
       </c>
@@ -800,7 +799,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>3</v>
       </c>
@@ -838,7 +837,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C16" s="1">
         <v>1</v>
       </c>
@@ -866,7 +865,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
         <v>2</v>
       </c>
@@ -890,7 +889,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
         <v>3</v>
       </c>
@@ -909,7 +908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>31</v>
       </c>
@@ -920,7 +919,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>32</v>
       </c>
@@ -939,11 +938,11 @@
       <c r="H21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="I21" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <v>1</v>
       </c>
@@ -956,7 +955,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="23" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <v>2</v>
       </c>
@@ -969,7 +968,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <v>3</v>
       </c>
@@ -982,279 +981,6 @@
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="3"/>
-      <c r="T28" s="3"/>
-      <c r="U28" s="3"/>
-      <c r="V28" s="3"/>
-    </row>
-    <row r="29" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
-      <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
-      <c r="V29" s="3"/>
-    </row>
-    <row r="30" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="3"/>
-      <c r="S30" s="3"/>
-      <c r="T30" s="3"/>
-      <c r="U30" s="3"/>
-      <c r="V30" s="3"/>
-    </row>
-    <row r="31" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="3"/>
-      <c r="S31" s="3"/>
-      <c r="T31" s="3"/>
-      <c r="U31" s="3"/>
-      <c r="V31" s="3"/>
-    </row>
-    <row r="32" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
-      <c r="R32" s="3"/>
-      <c r="S32" s="3"/>
-      <c r="T32" s="3"/>
-      <c r="U32" s="3"/>
-      <c r="V32" s="3"/>
-    </row>
-    <row r="33" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="3"/>
-      <c r="S33" s="3"/>
-      <c r="T33" s="3"/>
-      <c r="U33" s="3"/>
-      <c r="V33" s="3"/>
-    </row>
-    <row r="34" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
-      <c r="P34" s="3"/>
-      <c r="Q34" s="3"/>
-      <c r="R34" s="3"/>
-      <c r="S34" s="3"/>
-      <c r="T34" s="3"/>
-      <c r="U34" s="3"/>
-      <c r="V34" s="3"/>
-    </row>
-    <row r="35" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
-      <c r="P35" s="3"/>
-      <c r="Q35" s="3"/>
-      <c r="R35" s="3"/>
-      <c r="S35" s="3"/>
-      <c r="T35" s="3"/>
-      <c r="U35" s="3"/>
-      <c r="V35" s="3"/>
-    </row>
-    <row r="36" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
-      <c r="P36" s="3"/>
-      <c r="Q36" s="3"/>
-      <c r="R36" s="3"/>
-      <c r="S36" s="3"/>
-      <c r="T36" s="3"/>
-      <c r="U36" s="3"/>
-      <c r="V36" s="3"/>
-    </row>
-    <row r="37" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
-      <c r="R37" s="3"/>
-      <c r="S37" s="3"/>
-      <c r="T37" s="3"/>
-      <c r="U37" s="3"/>
-      <c r="V37" s="3"/>
-    </row>
-    <row r="38" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="3"/>
-      <c r="S38" s="3"/>
-      <c r="T38" s="3"/>
-      <c r="U38" s="3"/>
-      <c r="V38" s="3"/>
-    </row>
-    <row r="39" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-      <c r="S39" s="3"/>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
-      <c r="V39" s="3"/>
-    </row>
-    <row r="40" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="3"/>
-      <c r="R40" s="3"/>
-      <c r="S40" s="3"/>
-      <c r="T40" s="3"/>
-      <c r="U40" s="3"/>
-      <c r="V40" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>